<commit_message>
No changes, just removed filter from file
</commit_message>
<xml_diff>
--- a/Facilities masterlist.xlsx
+++ b/Facilities masterlist.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet 1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$I$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$I$96</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="328">
   <si>
     <t>22811 W 7 MILE RD</t>
   </si>
@@ -643,6 +643,369 @@
   </si>
   <si>
     <t>MEADOW OF HONOR APTS</t>
+  </si>
+  <si>
+    <t>2640 TRUMBULL ST</t>
+  </si>
+  <si>
+    <t>CATHOLIC WORKER DAY HOUSE</t>
+  </si>
+  <si>
+    <t>TRANSISIONAL HOUSING</t>
+  </si>
+  <si>
+    <t>4875 COPLIN ST</t>
+  </si>
+  <si>
+    <t>700 E GRAND BLVD</t>
+  </si>
+  <si>
+    <t>POSITIVE IMAGES</t>
+  </si>
+  <si>
+    <t>LTCF/SUD</t>
+  </si>
+  <si>
+    <t>MORTON MANOR</t>
+  </si>
+  <si>
+    <t>PABLO DAVIS</t>
+  </si>
+  <si>
+    <t>PASSION AND CARING HOME FOR THE ELDERLY</t>
+  </si>
+  <si>
+    <t>PHILLIP SIMS</t>
+  </si>
+  <si>
+    <t>PLYMOUTH SQUARE VILLAGE APTS</t>
+  </si>
+  <si>
+    <t>RESTORATION TOWERS</t>
+  </si>
+  <si>
+    <t>RIO VISTA</t>
+  </si>
+  <si>
+    <t>ROBERT HOLMES TEAMSTER HOUSING</t>
+  </si>
+  <si>
+    <t>SHAR ADMIN &amp; RESIDENTIAL TREATMENT - MAIN</t>
+  </si>
+  <si>
+    <t>RIVERTOWN ASSISTED LIVING</t>
+  </si>
+  <si>
+    <t>THE VILLAGE OF ST. MARTHA'S</t>
+  </si>
+  <si>
+    <t>THE VILLAGES OF ST. MARTHA'S</t>
+  </si>
+  <si>
+    <t>THOME RIVERTOWN NEIGHBORHOOD</t>
+  </si>
+  <si>
+    <t>QUALITY BEHAVIORAL HEALTH</t>
+  </si>
+  <si>
+    <t>VILLAGE CENTER</t>
+  </si>
+  <si>
+    <t>VILLAGE OF BETHANY MANOR</t>
+  </si>
+  <si>
+    <t>VILLAGE OF BRUSH PARK MANOR</t>
+  </si>
+  <si>
+    <t>VILLAGE OF OAKMAN MANOR</t>
+  </si>
+  <si>
+    <t>WOODBRIDGE SENIOR APARTMENTS II</t>
+  </si>
+  <si>
+    <t>20000 DEQUINDRE ST</t>
+  </si>
+  <si>
+    <t>9200 W VERNOR HWY</t>
+  </si>
+  <si>
+    <t>570 E GRAND BLVD</t>
+  </si>
+  <si>
+    <t>800 DICKERSON ST</t>
+  </si>
+  <si>
+    <t>20201 PLYMOUTH RD</t>
+  </si>
+  <si>
+    <t>16651 LAHSER RD</t>
+  </si>
+  <si>
+    <t>1250 18TH ST</t>
+  </si>
+  <si>
+    <t>5100 BRUSH ST</t>
+  </si>
+  <si>
+    <t>1852 W GRAND BLVD</t>
+  </si>
+  <si>
+    <t>250 MCDOUGALL ST</t>
+  </si>
+  <si>
+    <t>15801 JOY RD</t>
+  </si>
+  <si>
+    <t>15875 JOY RD</t>
+  </si>
+  <si>
+    <t>260 MCDOUGALL ST</t>
+  </si>
+  <si>
+    <t>751 E GRAND BLVD</t>
+  </si>
+  <si>
+    <t>901 PALLISTER ST</t>
+  </si>
+  <si>
+    <t>8737 14TH ST</t>
+  </si>
+  <si>
+    <t>2900 BRUSH ST</t>
+  </si>
+  <si>
+    <t>14000 WOODROW WILSON ST</t>
+  </si>
+  <si>
+    <t>1231 SELDEN ST</t>
+  </si>
+  <si>
+    <t>SUD</t>
+  </si>
+  <si>
+    <t>MIRACLE MANOR #3</t>
+  </si>
+  <si>
+    <t>MOM'S HEALING HANDS II</t>
+  </si>
+  <si>
+    <t>MOM'S HEALING HANDS, I</t>
+  </si>
+  <si>
+    <t>929 E GRAND BLVD</t>
+  </si>
+  <si>
+    <t>1027 E GRAND BLVD</t>
+  </si>
+  <si>
+    <t>975 E GRAND BLVD</t>
+  </si>
+  <si>
+    <t>AFC</t>
+  </si>
+  <si>
+    <t>PALMETTO AFC, LLC</t>
+  </si>
+  <si>
+    <t>PRECIOUSCARE 1</t>
+  </si>
+  <si>
+    <t>REGINAS HOME</t>
+  </si>
+  <si>
+    <t>ROSEBERRY AFC #2</t>
+  </si>
+  <si>
+    <t>ROSEBERRY AFC HOME #1</t>
+  </si>
+  <si>
+    <t>WOODINGHAM MANOR</t>
+  </si>
+  <si>
+    <t>7172 PALMETTO ST</t>
+  </si>
+  <si>
+    <t>7176 PALMETTO ST</t>
+  </si>
+  <si>
+    <t>12368 EVANSTON ST</t>
+  </si>
+  <si>
+    <t>139 TAYLOR ST</t>
+  </si>
+  <si>
+    <t>7184 PALMETTO ST</t>
+  </si>
+  <si>
+    <t>7182 PALMETTO ST</t>
+  </si>
+  <si>
+    <t>7161 PALMETTO ST</t>
+  </si>
+  <si>
+    <t>7167 PALMETTO ST</t>
+  </si>
+  <si>
+    <t>18461 WOODINGHAM ST</t>
+  </si>
+  <si>
+    <t>158 PINGREE ST</t>
+  </si>
+  <si>
+    <t>23001 NORFOLK ST</t>
+  </si>
+  <si>
+    <t>9298 WYOMING ST</t>
+  </si>
+  <si>
+    <t>18991 FENMORE ST</t>
+  </si>
+  <si>
+    <t>415 BURNS DR</t>
+  </si>
+  <si>
+    <t>7800 E JEFFERSON AVE</t>
+  </si>
+  <si>
+    <t>4386 CONNER ST</t>
+  </si>
+  <si>
+    <t>12041 ROSEMARY ST</t>
+  </si>
+  <si>
+    <t>7501 E JEFFERSON AVE</t>
+  </si>
+  <si>
+    <t>7601 E JEFFERSON AVE</t>
+  </si>
+  <si>
+    <t>1920 25TH ST</t>
+  </si>
+  <si>
+    <t>2925 RUSSEL ST</t>
+  </si>
+  <si>
+    <t>3646 MOUNT ELLIOTT ST</t>
+  </si>
+  <si>
+    <t>9341 AGNES ST</t>
+  </si>
+  <si>
+    <t>16800 WYOMING ST</t>
+  </si>
+  <si>
+    <t>3103 WIGHT ST</t>
+  </si>
+  <si>
+    <t>23001 W GRAND RIVER AVE</t>
+  </si>
+  <si>
+    <t>8600 CAMERON ST</t>
+  </si>
+  <si>
+    <t>14034 WOODROW WILSON ST</t>
+  </si>
+  <si>
+    <t>1556 KENDALL ST</t>
+  </si>
+  <si>
+    <t>1300 MARTIN LUTHER KING JR BLVD</t>
+  </si>
+  <si>
+    <t>2021 BLAINE ST</t>
+  </si>
+  <si>
+    <t>48 CHANDLER ST</t>
+  </si>
+  <si>
+    <t>430 E WARREN AVE</t>
+  </si>
+  <si>
+    <t>4100 W WARREN AVE</t>
+  </si>
+  <si>
+    <t>99 E FOREST AVE</t>
+  </si>
+  <si>
+    <t>3521 JOHN C LODGE FWY</t>
+  </si>
+  <si>
+    <t>NEW CENTER INN COMPANY</t>
+  </si>
+  <si>
+    <t>NORFOLK HOUSE</t>
+  </si>
+  <si>
+    <t>PHILLIPS CTH</t>
+  </si>
+  <si>
+    <t>ROSE CARE</t>
+  </si>
+  <si>
+    <t>W C TURNER I</t>
+  </si>
+  <si>
+    <t>OZIE LATRECE HOME</t>
+  </si>
+  <si>
+    <t>RIVER PARK VILLAGE</t>
+  </si>
+  <si>
+    <t>RIVER TOWERS</t>
+  </si>
+  <si>
+    <t>RIVERBEND TOWERS</t>
+  </si>
+  <si>
+    <t>SHERIDAN PLACE I</t>
+  </si>
+  <si>
+    <t>SHERIDAN PLACE II</t>
+  </si>
+  <si>
+    <t>SOUTHWEST HOUSING SOLUTIONS</t>
+  </si>
+  <si>
+    <t>TEAM WELLNESS CENTER</t>
+  </si>
+  <si>
+    <t>THE VERNON CENTER</t>
+  </si>
+  <si>
+    <t>THERESA MAXIS APARTMENTS</t>
+  </si>
+  <si>
+    <t>THOME RIVERTOWN ASSISTED LIVING</t>
+  </si>
+  <si>
+    <t>HOSPICE OF METRO DETROIT HOME HEALTH FAMILY SERVICES INC﻿</t>
+  </si>
+  <si>
+    <t>VANGUARD ELDERLY</t>
+  </si>
+  <si>
+    <t>VILLAGE OF WOODBRIDGE MANOR</t>
+  </si>
+  <si>
+    <t>VIRGINIA PARK MEADOWS</t>
+  </si>
+  <si>
+    <t>WARREN PLAZA APTS</t>
+  </si>
+  <si>
+    <t>WARREN WEST APTS</t>
+  </si>
+  <si>
+    <t>WILLIAMS PAVILION</t>
+  </si>
+  <si>
+    <t>WOODBRIDGE SENIOR VILLAGE APTS</t>
+  </si>
+  <si>
+    <t>Psychiatric center/Substance Abuse</t>
+  </si>
+  <si>
+    <t>TEAM MENTAL HEALTH WELLNESS</t>
   </si>
 </sst>
 </file>
@@ -686,7 +1049,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -694,11 +1057,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -712,6 +1090,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1010,11 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="B122" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,7 +1450,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +1471,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>48</v>
       </c>
@@ -1112,7 +1492,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>49</v>
       </c>
@@ -1133,7 +1513,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
@@ -1154,7 +1534,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1175,7 +1555,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>41</v>
       </c>
@@ -1196,7 +1576,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1217,7 +1597,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -1238,7 +1618,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -1259,7 +1639,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -1280,7 +1660,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
@@ -1301,7 +1681,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1322,7 +1702,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
@@ -1343,7 +1723,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1744,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
@@ -1385,7 +1765,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
@@ -1406,7 +1786,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>12</v>
       </c>
@@ -1427,7 +1807,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1448,7 +1828,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
@@ -1469,7 +1849,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1490,7 +1870,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>2</v>
       </c>
@@ -1511,7 +1891,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>6</v>
       </c>
@@ -1532,7 +1912,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>11</v>
       </c>
@@ -1553,7 +1933,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>43</v>
       </c>
@@ -1574,7 +1954,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1971,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>47</v>
       </c>
@@ -1608,7 +1988,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +2005,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>83</v>
       </c>
@@ -1642,7 +2022,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>84</v>
       </c>
@@ -1659,7 +2039,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>85</v>
       </c>
@@ -1676,7 +2056,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>99</v>
       </c>
@@ -1693,7 +2073,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>100</v>
       </c>
@@ -1710,7 +2090,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>86</v>
       </c>
@@ -1727,7 +2107,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>87</v>
       </c>
@@ -1744,7 +2124,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>101</v>
       </c>
@@ -1761,7 +2141,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>88</v>
       </c>
@@ -1778,7 +2158,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>89</v>
       </c>
@@ -1795,7 +2175,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>90</v>
       </c>
@@ -1812,7 +2192,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>91</v>
       </c>
@@ -1829,7 +2209,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>92</v>
       </c>
@@ -1846,7 +2226,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>102</v>
       </c>
@@ -1863,7 +2243,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>103</v>
       </c>
@@ -1880,7 +2260,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
         <v>14</v>
       </c>
@@ -1897,7 +2277,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>104</v>
       </c>
@@ -1914,7 +2294,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>93</v>
       </c>
@@ -1931,7 +2311,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>94</v>
       </c>
@@ -1948,7 +2328,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>95</v>
       </c>
@@ -1965,7 +2345,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>96</v>
       </c>
@@ -1982,7 +2362,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>105</v>
       </c>
@@ -1999,7 +2379,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>106</v>
       </c>
@@ -2016,7 +2396,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>97</v>
       </c>
@@ -2033,7 +2413,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>107</v>
       </c>
@@ -2050,7 +2430,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>108</v>
       </c>
@@ -2067,7 +2447,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
         <v>98</v>
       </c>
@@ -2084,7 +2464,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
         <v>109</v>
       </c>
@@ -2101,7 +2481,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>110</v>
       </c>
@@ -2118,7 +2498,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>111</v>
       </c>
@@ -2160,7 +2540,7 @@
         <v>148</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>50</v>
+        <v>259</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -2279,7 +2659,7 @@
         <v>150</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>50</v>
+        <v>259</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
@@ -2347,7 +2727,7 @@
         <v>151</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>50</v>
+        <v>259</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
@@ -2616,7 +2996,7 @@
         <v>203</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>50</v>
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
@@ -2641,14 +3021,701 @@
         <v>50</v>
       </c>
     </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B94" t="s">
+        <v>208</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>210</v>
+      </c>
+      <c r="B95" t="s">
+        <v>212</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>211</v>
+      </c>
+      <c r="B96" t="s">
+        <v>212</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>233</v>
+      </c>
+      <c r="B97" t="s">
+        <v>214</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>76</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>234</v>
+      </c>
+      <c r="B99" t="s">
+        <v>215</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>235</v>
+      </c>
+      <c r="B100" t="s">
+        <v>216</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>236</v>
+      </c>
+      <c r="B101" t="s">
+        <v>217</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>237</v>
+      </c>
+      <c r="B102" t="s">
+        <v>218</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>238</v>
+      </c>
+      <c r="B103" t="s">
+        <v>219</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>239</v>
+      </c>
+      <c r="B104" t="s">
+        <v>220</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>240</v>
+      </c>
+      <c r="B105" t="s">
+        <v>221</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>241</v>
+      </c>
+      <c r="B106" t="s">
+        <v>222</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>242</v>
+      </c>
+      <c r="B107" t="s">
+        <v>223</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>243</v>
+      </c>
+      <c r="B108" t="s">
+        <v>224</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>244</v>
+      </c>
+      <c r="B109" t="s">
+        <v>225</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>245</v>
+      </c>
+      <c r="B110" t="s">
+        <v>226</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>246</v>
+      </c>
+      <c r="B111" t="s">
+        <v>227</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>247</v>
+      </c>
+      <c r="B112" t="s">
+        <v>228</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>248</v>
+      </c>
+      <c r="B113" t="s">
+        <v>229</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>249</v>
+      </c>
+      <c r="B114" t="s">
+        <v>230</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>250</v>
+      </c>
+      <c r="B115" t="s">
+        <v>231</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>251</v>
+      </c>
+      <c r="B116" t="s">
+        <v>232</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>256</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>257</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>258</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>266</v>
+      </c>
+      <c r="B120" t="s">
+        <v>260</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>267</v>
+      </c>
+      <c r="B121" t="s">
+        <v>260</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>268</v>
+      </c>
+      <c r="B122" t="s">
+        <v>261</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>269</v>
+      </c>
+      <c r="B123" t="s">
+        <v>262</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>270</v>
+      </c>
+      <c r="B124" t="s">
+        <v>263</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>271</v>
+      </c>
+      <c r="B125" t="s">
+        <v>263</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>272</v>
+      </c>
+      <c r="B126" t="s">
+        <v>264</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>273</v>
+      </c>
+      <c r="B127" t="s">
+        <v>264</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>274</v>
+      </c>
+      <c r="B128" t="s">
+        <v>265</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>275</v>
+      </c>
+      <c r="B129" t="s">
+        <v>302</v>
+      </c>
+      <c r="C129" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>276</v>
+      </c>
+      <c r="B130" t="s">
+        <v>303</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>277</v>
+      </c>
+      <c r="B131" t="s">
+        <v>307</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>278</v>
+      </c>
+      <c r="B132" t="s">
+        <v>304</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>279</v>
+      </c>
+      <c r="B133" t="s">
+        <v>308</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>280</v>
+      </c>
+      <c r="B134" t="s">
+        <v>309</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>281</v>
+      </c>
+      <c r="B135" t="s">
+        <v>310</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>282</v>
+      </c>
+      <c r="B136" t="s">
+        <v>305</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>283</v>
+      </c>
+      <c r="B137" t="s">
+        <v>311</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>284</v>
+      </c>
+      <c r="B138" t="s">
+        <v>312</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>285</v>
+      </c>
+      <c r="B139" t="s">
+        <v>313</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>286</v>
+      </c>
+      <c r="B140" t="s">
+        <v>327</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>287</v>
+      </c>
+      <c r="B141" t="s">
+        <v>314</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>288</v>
+      </c>
+      <c r="B142" t="s">
+        <v>315</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>289</v>
+      </c>
+      <c r="B143" t="s">
+        <v>316</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>290</v>
+      </c>
+      <c r="B144" t="s">
+        <v>317</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>291</v>
+      </c>
+      <c r="B145" t="s">
+        <v>318</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>292</v>
+      </c>
+      <c r="B146" t="s">
+        <v>319</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>195</v>
+      </c>
+      <c r="B147" t="s">
+        <v>196</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>293</v>
+      </c>
+      <c r="B148" t="s">
+        <v>231</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>294</v>
+      </c>
+      <c r="B149" t="s">
+        <v>231</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>295</v>
+      </c>
+      <c r="B150" t="s">
+        <v>320</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>296</v>
+      </c>
+      <c r="B151" t="s">
+        <v>321</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>297</v>
+      </c>
+      <c r="B152" t="s">
+        <v>306</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>298</v>
+      </c>
+      <c r="B153" t="s">
+        <v>322</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>299</v>
+      </c>
+      <c r="B154" t="s">
+        <v>323</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>300</v>
+      </c>
+      <c r="B155" t="s">
+        <v>324</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>301</v>
+      </c>
+      <c r="B156" t="s">
+        <v>325</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I81">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="LTCF"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I96"/>
   <hyperlinks>
     <hyperlink ref="B35" r:id="rId1" display="https://www.bing.com/local?lid=YN427x401333935&amp;id=YN427x401333935&amp;q=Cots+Administrative+Offices&amp;name=Cots+Administrative+Offices&amp;cp=42.34511184692383%7e-83.05741882324219&amp;ppois=42.34511184692383_-83.05741882324219_Cots+Administrative+Offices&amp;FORM=SNAPST"/>
     <hyperlink ref="B48" r:id="rId2" display="https://www.bing.com/local?lid=YN873x10028322644708424806&amp;id=YN873x10028322644708424806&amp;q=Freedom+House+Detroit&amp;name=Freedom+House+Detroit&amp;cp=42.31310272216797%7e-83.11380004882812&amp;ppois=42.31310272216797_-83.11380004882812_Freedom+House+Detroit&amp;FORM=SNAPST"/>

</xml_diff>

<commit_message>
Added flag for 65+ and inpatient 65+. Fixed addresses in masterlist
</commit_message>
<xml_diff>
--- a/Facilities masterlist.xlsx
+++ b/Facilities masterlist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bivinsj\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bivinsj\Desktop\Case Pulls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24AE099F-F3CC-466B-9E13-14762BF53ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99A56DCD-5EF6-49BD-95A1-69775F4C5817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,32 @@
     <sheet name="Sheet 1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$I$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$I$208</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={177BB4A8-3265-4C1A-9EDD-D88A03F63D4E}</author>
+  </authors>
+  <commentList>
+    <comment ref="E209" authorId="0" shapeId="0" xr:uid="{177BB4A8-3265-4C1A-9EDD-D88A03F63D4E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Assuming this is where the DDC and Wayne County Juvenile Detention Facility should be</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="427">
   <si>
     <t>22811 W 7 MILE RD</t>
   </si>
@@ -151,9 +169,6 @@
     <t>464 E GRAND BLVD</t>
   </si>
   <si>
-    <t>845 E JEFFERSON AVE</t>
-  </si>
-  <si>
     <t>9146 WOODWARD AVE</t>
   </si>
   <si>
@@ -169,12 +184,6 @@
     <t>22355 W 8 MILE RD</t>
   </si>
   <si>
-    <t>5555 CONNER ST</t>
-  </si>
-  <si>
-    <t>5555 CONNER ST STE 2691</t>
-  </si>
-  <si>
     <t>LTCF</t>
   </si>
   <si>
@@ -535,9 +544,6 @@
     <t>Advantage Living Center-Samaritan</t>
   </si>
   <si>
-    <t>Ambassador, a Villa Center</t>
-  </si>
-  <si>
     <t>Beaconshire</t>
   </si>
   <si>
@@ -1310,6 +1316,12 @@
   </si>
   <si>
     <t>500 GRISWOLD ST</t>
+  </si>
+  <si>
+    <t>5555 Conner Street, 4th Floor</t>
+  </si>
+  <si>
+    <t>8045 E Jefferson</t>
   </si>
 </sst>
 </file>
@@ -1422,6 +1434,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Keith Kiama" id="{4196EDEA-D4CC-4B69-8675-96782CC345AE}" userId="S::kiamak@detroitmi.gov::ea63f6ea-f653-425b-8f47-f993b9a3ebf2" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1701,12 +1719,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E209" dT="2022-01-27T21:01:52.14" personId="{4196EDEA-D4CC-4B69-8675-96782CC345AE}" id="{177BB4A8-3265-4C1A-9EDD-D88A03F63D4E}">
+    <text>Assuming this is where the DDC and Wayne County Juvenile Detention Facility should be</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I213"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D213" sqref="D213"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1720,22 +1746,22 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -1749,14 +1775,14 @@
         <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -1770,14 +1796,14 @@
         <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1785,20 +1811,20 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>48</v>
+        <v>425</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -1806,20 +1832,20 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>49</v>
+        <v>426</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -1827,20 +1853,20 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1848,20 +1874,20 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -1869,20 +1895,20 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1890,20 +1916,20 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>119</v>
+        <v>169</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1911,20 +1937,20 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1932,20 +1958,20 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -1953,20 +1979,20 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1974,20 +2000,20 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>176</v>
+        <v>33</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1995,20 +2021,20 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -2016,20 +2042,20 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -2037,20 +2063,20 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -2058,20 +2084,20 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -2079,20 +2105,20 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -2100,20 +2126,20 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -2121,20 +2147,20 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>178</v>
+        <v>115</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -2142,20 +2168,20 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -2163,20 +2189,20 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -2184,20 +2210,20 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -2205,20 +2231,20 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -2226,20 +2252,20 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>182</v>
+        <v>118</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>45</v>
+        <v>417</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -2247,20 +2273,20 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>121</v>
+        <v>416</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -2268,20 +2294,20 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2289,34 +2315,30 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>421</v>
-      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>80</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -2327,13 +2349,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -2344,13 +2366,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -2361,13 +2383,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -2378,13 +2400,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -2395,13 +2417,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -2412,13 +2434,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -2429,13 +2451,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -2446,13 +2468,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2463,13 +2485,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2480,13 +2502,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2497,13 +2519,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -2514,13 +2536,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -2531,13 +2553,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2548,13 +2570,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -2565,13 +2587,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -2582,13 +2604,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -2599,13 +2621,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2616,13 +2638,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -2633,13 +2655,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -2650,13 +2672,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -2667,13 +2689,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -2684,13 +2706,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -2701,13 +2723,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -2718,13 +2740,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -2735,13 +2757,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -2752,13 +2774,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -2769,13 +2791,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -2786,13 +2808,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -2803,13 +2825,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -2819,14 +2841,14 @@
       <c r="I58" s="6"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>79</v>
+      <c r="A59" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -2837,13 +2859,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>50</v>
+        <v>254</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
@@ -2854,13 +2876,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>258</v>
+        <v>47</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -2871,13 +2893,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -2888,13 +2910,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
@@ -2905,13 +2927,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
@@ -2922,13 +2944,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
@@ -2939,13 +2961,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
@@ -2956,13 +2978,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>50</v>
+        <v>254</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
@@ -2973,13 +2995,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>258</v>
+        <v>47</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
@@ -2990,13 +3012,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
@@ -3007,13 +3029,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -3023,14 +3045,14 @@
       <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71" s="4" t="s">
-        <v>136</v>
+      <c r="A71" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>50</v>
+        <v>254</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
@@ -3041,13 +3063,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>258</v>
+        <v>47</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
@@ -3058,13 +3080,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
@@ -3074,14 +3096,14 @@
       <c r="I73" s="6"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
-        <v>139</v>
+      <c r="A74" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
@@ -3091,14 +3113,14 @@
       <c r="I74" s="6"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="s">
-        <v>140</v>
+      <c r="A75" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
@@ -3108,14 +3130,14 @@
       <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
-        <v>141</v>
+      <c r="A76" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
@@ -3125,14 +3147,14 @@
       <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A77" s="4" t="s">
-        <v>142</v>
+      <c r="A77" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
@@ -3143,13 +3165,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
@@ -3159,14 +3181,14 @@
       <c r="I78" s="6"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
-        <v>144</v>
+      <c r="A79" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
@@ -3177,13 +3199,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
@@ -3192,158 +3214,152 @@
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>167</v>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" t="s">
+        <v>179</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>181</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B83" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>184</v>
       </c>
-      <c r="B82" t="s">
-        <v>183</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+      <c r="B84" t="s">
         <v>185</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="8" t="s">
+      <c r="C84" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>187</v>
+      </c>
+      <c r="B85" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B84" t="s">
-        <v>187</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="C85" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>189</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+      <c r="C86" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B87" t="s">
         <v>191</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="8" t="s">
+      <c r="C87" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>193</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B87" t="s">
-        <v>193</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="8" t="s">
+      <c r="C88" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B88" t="s">
-        <v>195</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+      <c r="C89" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>197</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B90" t="s">
+        <v>198</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B91" t="s">
         <v>196</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A90" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+      <c r="C91" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>200</v>
+      </c>
+      <c r="B92" t="s">
         <v>201</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C92" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="4" t="s">
+      <c r="B93" t="s">
         <v>203</v>
       </c>
-      <c r="B92" t="s">
-        <v>200</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="C93" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B93" t="s">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>205</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="B94" t="s">
         <v>207</v>
@@ -3352,1331 +3368,1320 @@
         <v>208</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>206</v>
+      </c>
+      <c r="B95" t="s">
+        <v>207</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>228</v>
+      </c>
+      <c r="B96" t="s">
         <v>209</v>
       </c>
-      <c r="B95" t="s">
-        <v>211</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>210</v>
-      </c>
-      <c r="B96" t="s">
-        <v>211</v>
-      </c>
       <c r="C96" s="3" t="s">
-        <v>212</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B97" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B98" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B99" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B100" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B101" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B102" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B103" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B104" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B105" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B106" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B107" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B108" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B109" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>50</v>
+        <v>247</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B110" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>251</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B111" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B112" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B113" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B114" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>250</v>
-      </c>
-      <c r="B115" t="s">
-        <v>231</v>
+        <v>251</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>50</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>256</v>
-      </c>
-      <c r="B117" s="7" t="s">
         <v>253</v>
       </c>
+      <c r="B117" s="9" t="s">
+        <v>250</v>
+      </c>
       <c r="C117" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>257</v>
-      </c>
-      <c r="B118" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B118" t="s">
+        <v>255</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B119" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B120" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B121" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B122" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B123" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B124" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B125" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B126" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B127" t="s">
-        <v>264</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="C127" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B128" t="s">
-        <v>301</v>
-      </c>
-      <c r="C128" t="s">
-        <v>50</v>
+        <v>298</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B129" t="s">
         <v>302</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B130" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B131" t="s">
         <v>303</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B132" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B133" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B134" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B135" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B136" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B137" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>50</v>
+        <v>204</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B138" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>208</v>
+        <v>321</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B139" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B140" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>325</v>
+        <v>47</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B141" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B142" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B144" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B145" t="s">
-        <v>318</v>
+        <v>226</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B146" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B147" t="s">
-        <v>230</v>
+        <v>315</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B148" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B149" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B150" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B151" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B152" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B153" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="B154" t="s">
         <v>324</v>
       </c>
-      <c r="C154" s="6" t="s">
-        <v>50</v>
+      <c r="C154" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B155" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C155" t="s">
-        <v>51</v>
+        <v>247</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B156" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C156" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B157" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C157" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B158" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C158" t="s">
-        <v>251</v>
+        <v>48</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B159" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C159" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B160" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C160" t="s">
-        <v>51</v>
+        <v>247</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B161" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C161" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B162" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C162" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
+        <v>340</v>
+      </c>
+      <c r="B163" t="s">
+        <v>341</v>
+      </c>
+      <c r="C163" t="s">
         <v>342</v>
-      </c>
-      <c r="B163" t="s">
-        <v>343</v>
-      </c>
-      <c r="C163" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
+        <v>343</v>
+      </c>
+      <c r="B164" t="s">
         <v>344</v>
       </c>
-      <c r="B164" t="s">
-        <v>345</v>
-      </c>
       <c r="C164" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B165" t="s">
-        <v>348</v>
+        <v>222</v>
       </c>
       <c r="C165" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B166" t="s">
-        <v>226</v>
+        <v>347</v>
       </c>
       <c r="C166" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B167" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="C167" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B168" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="C168" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B169" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C169" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B170" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C170" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B171" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C171" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B172" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C172" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B173" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C173" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B174" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C174" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B175" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C175" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B176" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C176" t="s">
-        <v>251</v>
+        <v>48</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B177" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C177" t="s">
-        <v>51</v>
+        <v>342</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B178" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C178" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B179" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C179" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B180" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C180" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B181" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C181" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B182" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C182" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B183" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C183" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B184" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C184" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B185" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="C185" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B186" t="s">
-        <v>368</v>
+        <v>383</v>
       </c>
       <c r="C186" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B187" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C187" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B188" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C188" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B189" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C189" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B190" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C190" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B191" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C191" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B192" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C192" t="s">
-        <v>251</v>
+        <v>48</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B193" t="s">
-        <v>396</v>
+        <v>222</v>
       </c>
       <c r="C193" t="s">
-        <v>51</v>
+        <v>247</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B194" t="s">
-        <v>226</v>
+        <v>392</v>
       </c>
       <c r="C194" t="s">
-        <v>251</v>
+        <v>48</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B195" t="s">
-        <v>396</v>
+        <v>222</v>
       </c>
       <c r="C195" t="s">
-        <v>51</v>
+        <v>247</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B196" t="s">
-        <v>226</v>
+        <v>326</v>
       </c>
       <c r="C196" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B197" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C197" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B198" t="s">
-        <v>330</v>
+        <v>399</v>
       </c>
       <c r="C198" t="s">
-        <v>251</v>
+        <v>48</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B199" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C199" t="s">
-        <v>51</v>
+        <v>342</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B200" t="s">
-        <v>405</v>
+        <v>326</v>
       </c>
       <c r="C200" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B201" t="s">
-        <v>330</v>
+        <v>404</v>
       </c>
       <c r="C201" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B202" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C202" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B203" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C203" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B204" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C204" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B205" t="s">
-        <v>412</v>
+        <v>222</v>
       </c>
       <c r="C205" t="s">
-        <v>346</v>
+        <v>247</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B206" t="s">
-        <v>226</v>
+        <v>412</v>
       </c>
       <c r="C206" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B207" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C207" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B208" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C208" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>419</v>
       </c>
-      <c r="B209" t="s">
-        <v>418</v>
-      </c>
-      <c r="C209" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B209" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="C209" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
+        <v>420</v>
+      </c>
+      <c r="B210" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="D210" s="6"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
         <v>423</v>
       </c>
-      <c r="B210" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="C210" s="6" t="s">
+      <c r="B211" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="C211" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="D211" s="6"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>424</v>
+      </c>
+      <c r="B212" s="10" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A211" t="s">
-        <v>424</v>
-      </c>
-      <c r="B211" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="C211" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="D211" s="6"/>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A212" t="s">
-        <v>427</v>
-      </c>
-      <c r="B212" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="D212" s="6"/>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A213" t="s">
-        <v>428</v>
-      </c>
-      <c r="B213" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="C213" t="s">
-        <v>421</v>
+      <c r="C212" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I209" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1" display="https://www.bing.com/local?lid=YN427x401333935&amp;id=YN427x401333935&amp;q=Cots+Administrative+Offices&amp;name=Cots+Administrative+Offices&amp;cp=42.34511184692383%7e-83.05741882324219&amp;ppois=42.34511184692383_-83.05741882324219_Cots+Administrative+Offices&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B48" r:id="rId2" display="https://www.bing.com/local?lid=YN873x10028322644708424806&amp;id=YN873x10028322644708424806&amp;q=Freedom+House+Detroit&amp;name=Freedom+House+Detroit&amp;cp=42.31310272216797%7e-83.11380004882812&amp;ppois=42.31310272216797_-83.11380004882812_Freedom+House+Detroit&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B47" r:id="rId3" display="https://www.bing.com/local?lid=YN427x7697390&amp;id=YN427x7697390&amp;q=Faith+Clinic&amp;name=Faith+Clinic&amp;cp=42.40123748779297%7e-82.98211669921875&amp;ppois=42.40123748779297_-82.98211669921875_Faith+Clinic&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B38" r:id="rId4" display="https://www.bing.com/maps?cp=42.33583068847656%7e-83.08840942382812&amp;name=Covenant+House&amp;where1=2959+Martin+Luther+King+Jr+Blvd%2c+Detroit%2c+MI+48208&amp;ppois=42.33583068847656_-83.08840942382812_Covenant+House" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B55" r:id="rId5" display="https://www.bing.com/local?lid=YN873x15269134723373995179&amp;id=YN873x15269134723373995179&amp;q=Neighborhood+Service+Organization&amp;name=Neighborhood+Service+Organization&amp;cp=42.40291976928711%7e-83.11402130126953&amp;ppois=42.40291976928711_-83.11402130126953_Neighborhood+Service+Organization&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B49" r:id="rId6" display="https://www.bing.com/local?lid=YN427x7706995&amp;id=YN427x7706995&amp;q=Interim+House&amp;name=Interim+House&amp;cp=42.414180755615234%7e-83.1522445678711&amp;ppois=42.414180755615234_-83.1522445678711_Interim+House&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B33" r:id="rId7" display="https://www.bing.com/local?lid=YN427x401333935&amp;id=YN427x401333935&amp;q=Cots+Administrative+Offices&amp;name=Cots+Administrative+Offices&amp;cp=42.34511184692383%7e-83.05741882324219&amp;ppois=42.34511184692383_-83.05741882324219_Cots+Administrative+Offices&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B34" r:id="rId8" display="https://www.bing.com/local?lid=YN427x401333935&amp;id=YN427x401333935&amp;q=Cots+Administrative+Offices&amp;name=Cots+Administrative+Offices&amp;cp=42.34511184692383%7e-83.05741882324219&amp;ppois=42.34511184692383_-83.05741882324219_Cots+Administrative+Offices&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B37" r:id="rId9" display="https://www.bing.com/maps?cp=42.33583068847656%7e-83.08840942382812&amp;name=Covenant+House&amp;where1=2959+Martin+Luther+King+Jr+Blvd%2c+Detroit%2c+MI+48208&amp;ppois=42.33583068847656_-83.08840942382812_Covenant+House" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B34" r:id="rId1" display="https://www.bing.com/local?lid=YN427x401333935&amp;id=YN427x401333935&amp;q=Cots+Administrative+Offices&amp;name=Cots+Administrative+Offices&amp;cp=42.34511184692383%7e-83.05741882324219&amp;ppois=42.34511184692383_-83.05741882324219_Cots+Administrative+Offices&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B47" r:id="rId2" display="https://www.bing.com/local?lid=YN873x10028322644708424806&amp;id=YN873x10028322644708424806&amp;q=Freedom+House+Detroit&amp;name=Freedom+House+Detroit&amp;cp=42.31310272216797%7e-83.11380004882812&amp;ppois=42.31310272216797_-83.11380004882812_Freedom+House+Detroit&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B46" r:id="rId3" display="https://www.bing.com/local?lid=YN427x7697390&amp;id=YN427x7697390&amp;q=Faith+Clinic&amp;name=Faith+Clinic&amp;cp=42.40123748779297%7e-82.98211669921875&amp;ppois=42.40123748779297_-82.98211669921875_Faith+Clinic&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B37" r:id="rId4" display="https://www.bing.com/maps?cp=42.33583068847656%7e-83.08840942382812&amp;name=Covenant+House&amp;where1=2959+Martin+Luther+King+Jr+Blvd%2c+Detroit%2c+MI+48208&amp;ppois=42.33583068847656_-83.08840942382812_Covenant+House" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B54" r:id="rId5" display="https://www.bing.com/local?lid=YN873x15269134723373995179&amp;id=YN873x15269134723373995179&amp;q=Neighborhood+Service+Organization&amp;name=Neighborhood+Service+Organization&amp;cp=42.40291976928711%7e-83.11402130126953&amp;ppois=42.40291976928711_-83.11402130126953_Neighborhood+Service+Organization&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B48" r:id="rId6" display="https://www.bing.com/local?lid=YN427x7706995&amp;id=YN427x7706995&amp;q=Interim+House&amp;name=Interim+House&amp;cp=42.414180755615234%7e-83.1522445678711&amp;ppois=42.414180755615234_-83.1522445678711_Interim+House&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B32" r:id="rId7" display="https://www.bing.com/local?lid=YN427x401333935&amp;id=YN427x401333935&amp;q=Cots+Administrative+Offices&amp;name=Cots+Administrative+Offices&amp;cp=42.34511184692383%7e-83.05741882324219&amp;ppois=42.34511184692383_-83.05741882324219_Cots+Administrative+Offices&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B33" r:id="rId8" display="https://www.bing.com/local?lid=YN427x401333935&amp;id=YN427x401333935&amp;q=Cots+Administrative+Offices&amp;name=Cots+Administrative+Offices&amp;cp=42.34511184692383%7e-83.05741882324219&amp;ppois=42.34511184692383_-83.05741882324219_Cots+Administrative+Offices&amp;FORM=SNAPST" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B36" r:id="rId9" display="https://www.bing.com/maps?cp=42.33583068847656%7e-83.08840942382812&amp;name=Covenant+House&amp;where1=2959+Martin+Luther+King+Jr+Blvd%2c+Detroit%2c+MI+48208&amp;ppois=42.33583068847656_-83.08840942382812_Covenant+House" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>